<commit_message>
Corrected error in entry
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clorange\Dropbox\CLD\Orange House\Happy Hour\Denver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\CLD\Orange House\Happy Hour\Denver\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B753521-E5B0-48FB-86E5-66F7A62A68F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$290</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$C$1:$C$282</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3902,10 +3904,6 @@
     <t>$4 draft specials and $6 specialty 'Tails and select wines; $6 small plates or $15 for three (served at the Counter)</t>
   </si>
   <si>
-    <t>Half off all glasses of wine &lt;br&gt; Diebolt Brewery Anton Francois French Ale 3.00 &lt;br&gt; Cocktail of the day  6.00 &lt;br&gt;Moules 9.50&lt;br&gt;Cheese Burger 9.50&lt;br&gt;Pate Maison 5.50&lt;br&gt;Chicken Liver Mousse 6.50&lt;br&gt;
-Soupe a lOignon 5.00&lt;br&gt;Pommes Frites 3.00&lt;br&gt;Oozy and Boozy 9.00&lt;br&gt;Just Oozy 6.00&lt;br&gt;Socca Frites 3.50&lt;br&gt;Crispy Shrimp 5.00&lt;br&gt;</t>
-  </si>
-  <si>
     <t>4151 E. County Line Rd. Unit G Centennial CO</t>
   </si>
   <si>
@@ -3928,13 +3926,16 @@
   </si>
   <si>
     <t>2-for-1 wells, house wines and select domestic drafts, $1 off all craft and imported draft beers, and $4 Fireball shots; $7 snack menu &lt;br&gt;Daily food specials&lt;br&gt;Weekend drink specials 1pm-10pm</t>
+  </si>
+  <si>
+    <t>Half off all glasses of wine &lt;br&gt; Diebolt Brewery Anton Francois French Ale 3.00 &lt;br&gt; Cocktail of the day  6.00 &lt;br&gt;Moules 9.50&lt;br&gt;Cheese Burger 9.50&lt;br&gt;Pate Maison 5.50&lt;br&gt;Chicken Liver Mousse 6.50&lt;br&gt;Soupe a lOignon 5.00&lt;br&gt;Pommes Frites 3.00&lt;br&gt;Oozy and Boozy 9.00&lt;br&gt;Just Oozy 6.00&lt;br&gt;Socca Frites 3.50&lt;br&gt;Crispy Shrimp 5.00&lt;br&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="34" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4560,12 +4561,12 @@
     <cellStyle name="40% - Accent4" xfId="28" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent5" xfId="31" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent6" xfId="34" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="37"/>
-    <cellStyle name="60% - Accent2" xfId="38"/>
-    <cellStyle name="60% - Accent3" xfId="39"/>
-    <cellStyle name="60% - Accent4" xfId="40"/>
-    <cellStyle name="60% - Accent5" xfId="41"/>
-    <cellStyle name="60% - Accent6" xfId="42"/>
+    <cellStyle name="60% - Accent1" xfId="37" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2" xfId="38" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3" xfId="39" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4" xfId="40" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5" xfId="41" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6" xfId="42" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Accent1" xfId="17" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="23" builtinId="37" customBuiltin="1"/>
@@ -4584,11 +4585,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Input" xfId="8" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="11" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36"/>
+    <cellStyle name="Neutral" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="14" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="9" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="35"/>
+    <cellStyle name="Title" xfId="35" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="13" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -4617,7 +4618,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -4929,39 +4930,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BL316"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" customWidth="1"/>
     <col min="4" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" customWidth="1"/>
+    <col min="7" max="7" width="46.7265625" customWidth="1"/>
     <col min="8" max="35" width="6" customWidth="1"/>
-    <col min="36" max="36" width="10.28515625" customWidth="1"/>
-    <col min="37" max="37" width="10.85546875" customWidth="1"/>
-    <col min="38" max="38" width="13.5703125" customWidth="1"/>
+    <col min="36" max="36" width="10.26953125" customWidth="1"/>
+    <col min="37" max="37" width="10.81640625" customWidth="1"/>
+    <col min="38" max="38" width="13.54296875" customWidth="1"/>
     <col min="39" max="39" width="13" customWidth="1"/>
-    <col min="40" max="42" width="10.28515625" customWidth="1"/>
-    <col min="43" max="43" width="15.85546875" customWidth="1"/>
-    <col min="44" max="49" width="8.7109375" customWidth="1"/>
-    <col min="50" max="50" width="90.5703125" customWidth="1"/>
-    <col min="51" max="51" width="5.5703125" customWidth="1"/>
-    <col min="52" max="52" width="8.7109375" customWidth="1"/>
-    <col min="53" max="53" width="10.140625" customWidth="1"/>
-    <col min="54" max="55" width="8.7109375" customWidth="1"/>
-    <col min="56" max="56" width="11.42578125" customWidth="1"/>
-    <col min="57" max="57" width="53.5703125" customWidth="1"/>
-    <col min="58" max="58" width="18.5703125" customWidth="1"/>
+    <col min="40" max="42" width="10.26953125" customWidth="1"/>
+    <col min="43" max="43" width="15.81640625" customWidth="1"/>
+    <col min="44" max="49" width="8.7265625" customWidth="1"/>
+    <col min="50" max="50" width="90.54296875" customWidth="1"/>
+    <col min="51" max="51" width="5.54296875" customWidth="1"/>
+    <col min="52" max="52" width="8.7265625" customWidth="1"/>
+    <col min="53" max="53" width="10.1796875" customWidth="1"/>
+    <col min="54" max="55" width="8.7265625" customWidth="1"/>
+    <col min="56" max="56" width="11.453125" customWidth="1"/>
+    <col min="57" max="57" width="53.54296875" customWidth="1"/>
+    <col min="58" max="58" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:64" ht="18.75" customHeight="1">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -5129,7 +5130,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:64" ht="18.75" customHeight="1">
       <c r="B2" t="s">
         <v>165</v>
       </c>
@@ -5327,7 +5328,7 @@
       </c>
       <c r="BL2" s="7"/>
     </row>
-    <row r="3" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:64" ht="18.75" customHeight="1">
       <c r="B3" t="s">
         <v>1129</v>
       </c>
@@ -5517,7 +5518,7 @@
       </c>
       <c r="BL3" s="7"/>
     </row>
-    <row r="4" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:64" ht="18.75" customHeight="1">
       <c r="B4" t="s">
         <v>938</v>
       </c>
@@ -5714,7 +5715,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:64" ht="18.75" customHeight="1">
       <c r="B5" t="s">
         <v>938</v>
       </c>
@@ -5907,7 +5908,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:64" ht="18.75" customHeight="1">
       <c r="B6" t="s">
         <v>867</v>
       </c>
@@ -6112,7 +6113,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:64" ht="18.75" customHeight="1">
       <c r="B7" t="s">
         <v>1104</v>
       </c>
@@ -6313,7 +6314,7 @@
         <v>[39.7549,-104.977679],</v>
       </c>
     </row>
-    <row r="8" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:64" ht="18.75" customHeight="1">
       <c r="B8" t="s">
         <v>166</v>
       </c>
@@ -6522,7 +6523,7 @@
       </c>
       <c r="BL8" s="7"/>
     </row>
-    <row r="9" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:64" ht="18.75" customHeight="1">
       <c r="B9" t="s">
         <v>1180</v>
       </c>
@@ -6723,7 +6724,7 @@
         <v>[39.76874,-104.9798],</v>
       </c>
     </row>
-    <row r="10" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:64" ht="18.75" customHeight="1">
       <c r="B10" t="s">
         <v>59</v>
       </c>
@@ -6929,7 +6930,7 @@
       </c>
       <c r="BL10" s="7"/>
     </row>
-    <row r="11" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:64" ht="18.75" customHeight="1">
       <c r="B11" t="s">
         <v>231</v>
       </c>
@@ -7123,7 +7124,7 @@
       </c>
       <c r="BL11" s="7"/>
     </row>
-    <row r="12" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:64" ht="18.75" customHeight="1">
       <c r="B12" t="s">
         <v>246</v>
       </c>
@@ -7332,7 +7333,7 @@
       </c>
       <c r="BL12" s="7"/>
     </row>
-    <row r="13" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:64" ht="18.75" customHeight="1">
       <c r="B13" t="s">
         <v>1217</v>
       </c>
@@ -7541,7 +7542,7 @@
       </c>
       <c r="BL13" s="7"/>
     </row>
-    <row r="14" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:64" ht="18.75" customHeight="1">
       <c r="B14" t="s">
         <v>1146</v>
       </c>
@@ -7742,7 +7743,7 @@
         <v>[39.75426,-104.99066],</v>
       </c>
     </row>
-    <row r="15" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:64" ht="18.75" customHeight="1">
       <c r="B15" t="s">
         <v>914</v>
       </c>
@@ -7935,7 +7936,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:64" ht="18.75" customHeight="1">
       <c r="B16" t="s">
         <v>1150</v>
       </c>
@@ -8136,7 +8137,7 @@
         <v>[39.72549,-104.97929],</v>
       </c>
     </row>
-    <row r="17" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:64" ht="18.75" customHeight="1">
       <c r="B17" t="s">
         <v>834</v>
       </c>
@@ -8296,7 +8297,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:64" ht="18.75" customHeight="1">
       <c r="B18" t="s">
         <v>846</v>
       </c>
@@ -8489,7 +8490,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:64" ht="18.75" customHeight="1">
       <c r="B19" t="s">
         <v>60</v>
       </c>
@@ -8695,7 +8696,7 @@
       </c>
       <c r="BL19" s="7"/>
     </row>
-    <row r="20" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:64" ht="18.75" customHeight="1">
       <c r="B20" t="s">
         <v>926</v>
       </c>
@@ -8897,7 +8898,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:64" ht="18.75" customHeight="1">
       <c r="B21" t="s">
         <v>61</v>
       </c>
@@ -9058,7 +9059,7 @@
       </c>
       <c r="BL21" s="7"/>
     </row>
-    <row r="22" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:64" ht="18.75" customHeight="1">
       <c r="B22" t="s">
         <v>236</v>
       </c>
@@ -9222,7 +9223,7 @@
       </c>
       <c r="BL22" s="7"/>
     </row>
-    <row r="23" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:64" ht="18.75" customHeight="1">
       <c r="B23" t="s">
         <v>62</v>
       </c>
@@ -9428,7 +9429,7 @@
       </c>
       <c r="BL23" s="7"/>
     </row>
-    <row r="24" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:64" ht="18.75" customHeight="1">
       <c r="B24" s="1" t="s">
         <v>850</v>
       </c>
@@ -9585,7 +9586,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:64" ht="18.75" customHeight="1">
       <c r="B25" t="s">
         <v>63</v>
       </c>
@@ -9791,7 +9792,7 @@
       </c>
       <c r="BL25" s="7"/>
     </row>
-    <row r="26" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:64" ht="18.75" customHeight="1">
       <c r="B26" t="s">
         <v>64</v>
       </c>
@@ -9997,7 +9998,7 @@
       </c>
       <c r="BL26" s="7"/>
     </row>
-    <row r="27" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:64" ht="18.75" customHeight="1">
       <c r="B27" t="s">
         <v>65</v>
       </c>
@@ -10203,7 +10204,7 @@
       </c>
       <c r="BL27" s="7"/>
     </row>
-    <row r="28" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:64" ht="18.75" customHeight="1">
       <c r="B28" t="s">
         <v>892</v>
       </c>
@@ -10396,7 +10397,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:64" ht="18.75" customHeight="1">
       <c r="B29" t="s">
         <v>912</v>
       </c>
@@ -10589,7 +10590,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:64" ht="18.75" customHeight="1">
       <c r="B30" t="s">
         <v>888</v>
       </c>
@@ -10749,7 +10750,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:64" ht="18.75" customHeight="1">
       <c r="B31" t="s">
         <v>167</v>
       </c>
@@ -10949,7 +10950,7 @@
       </c>
       <c r="BL31" s="7"/>
     </row>
-    <row r="32" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:64" ht="18.75" customHeight="1">
       <c r="B32" t="s">
         <v>248</v>
       </c>
@@ -11113,7 +11114,7 @@
       </c>
       <c r="BL32" s="7"/>
     </row>
-    <row r="33" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:64" ht="18.75" customHeight="1">
       <c r="B33" t="s">
         <v>168</v>
       </c>
@@ -11307,7 +11308,7 @@
       </c>
       <c r="BL33" s="7"/>
     </row>
-    <row r="34" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:64" ht="18.75" customHeight="1">
       <c r="B34" t="s">
         <v>1123</v>
       </c>
@@ -11463,7 +11464,7 @@
         <v>[39.604065,-104.708484],</v>
       </c>
     </row>
-    <row r="35" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:64" ht="18.75" customHeight="1">
       <c r="B35" t="s">
         <v>169</v>
       </c>
@@ -11657,7 +11658,7 @@
       </c>
       <c r="BL35" s="7"/>
     </row>
-    <row r="36" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:64" ht="18.75" customHeight="1">
       <c r="B36" t="s">
         <v>1260</v>
       </c>
@@ -11843,7 +11844,7 @@
         <v>[39.76944,-104.97676],</v>
       </c>
     </row>
-    <row r="37" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:64" ht="18.75" customHeight="1">
       <c r="B37" t="s">
         <v>239</v>
       </c>
@@ -11899,7 +11900,7 @@
         <v>423</v>
       </c>
       <c r="V37" s="8" t="s">
-        <v>1289</v>
+        <v>1297</v>
       </c>
       <c r="W37">
         <f t="shared" si="0"/>
@@ -12002,8 +12003,7 @@
         <v>{
     'name': "Bistro Vendome",
     'area': "larimer",'hours': {
-      'sunday-start':"1500", 'sunday-end':"1700", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1500", 'saturday-end':"1700"},  'description': "Half off all glasses of wine &lt;br&gt; Diebolt Brewery Anton Francois French Ale 3.00 &lt;br&gt; Cocktail of the day  6.00 &lt;br&gt;Moules 9.50&lt;br&gt;Cheese Burger 9.50&lt;br&gt;Pate Maison 5.50&lt;br&gt;Chicken Liver Mousse 6.50&lt;br&gt;
-Soupe a lOignon 5.00&lt;br&gt;Pommes Frites 3.00&lt;br&gt;Oozy and Boozy 9.00&lt;br&gt;Just Oozy 6.00&lt;br&gt;Socca Frites 3.50&lt;br&gt;Crispy Shrimp 5.00&lt;br&gt;", 'link':"http://www.bistrovendome.com/", 'pricing':"med",   'phone-number': "", 'address': "1705, 1420 Larimer St, Denver, CO ", 'other-amenities': ['outside','',''], 'has-drink':true, 'has-food':true},</v>
+      'sunday-start':"1500", 'sunday-end':"1700", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1500", 'saturday-end':"1700"},  'description': "Half off all glasses of wine &lt;br&gt; Diebolt Brewery Anton Francois French Ale 3.00 &lt;br&gt; Cocktail of the day  6.00 &lt;br&gt;Moules 9.50&lt;br&gt;Cheese Burger 9.50&lt;br&gt;Pate Maison 5.50&lt;br&gt;Chicken Liver Mousse 6.50&lt;br&gt;Soupe a lOignon 5.00&lt;br&gt;Pommes Frites 3.00&lt;br&gt;Oozy and Boozy 9.00&lt;br&gt;Just Oozy 6.00&lt;br&gt;Socca Frites 3.50&lt;br&gt;Crispy Shrimp 5.00&lt;br&gt;", 'link':"http://www.bistrovendome.com/", 'pricing':"med",   'phone-number': "", 'address': "1705, 1420 Larimer St, Denver, CO ", 'other-amenities': ['outside','',''], 'has-drink':true, 'has-food':true},</v>
       </c>
       <c r="AY37" t="str">
         <f t="shared" si="22"/>
@@ -12053,7 +12053,7 @@
       </c>
       <c r="BL37" s="7"/>
     </row>
-    <row r="38" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:64" ht="18.75" customHeight="1">
       <c r="B38" t="s">
         <v>929</v>
       </c>
@@ -12258,7 +12258,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:64" ht="18.75" customHeight="1">
       <c r="B39" t="s">
         <v>66</v>
       </c>
@@ -12452,7 +12452,7 @@
       </c>
       <c r="BL39" s="7"/>
     </row>
-    <row r="40" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:64" ht="18.75" customHeight="1">
       <c r="B40" t="s">
         <v>170</v>
       </c>
@@ -12646,7 +12646,7 @@
       </c>
       <c r="BL40" s="7"/>
     </row>
-    <row r="41" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:64" ht="18.75" customHeight="1">
       <c r="B41" t="s">
         <v>171</v>
       </c>
@@ -12657,7 +12657,7 @@
         <v>1061</v>
       </c>
       <c r="G41" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="J41">
         <v>1500</v>
@@ -12690,7 +12690,7 @@
         <v>1800</v>
       </c>
       <c r="V41" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="W41" t="str">
         <f t="shared" si="0"/>
@@ -12840,7 +12840,7 @@
       </c>
       <c r="BL41" s="7"/>
     </row>
-    <row r="42" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:64" ht="18.75" customHeight="1">
       <c r="B42" t="s">
         <v>1183</v>
       </c>
@@ -13041,7 +13041,7 @@
         <v>[39.75134,-105.00048],</v>
       </c>
     </row>
-    <row r="43" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:64" ht="18.75" customHeight="1">
       <c r="B43" t="s">
         <v>67</v>
       </c>
@@ -13097,7 +13097,7 @@
         <v>421</v>
       </c>
       <c r="V43" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="W43">
         <f t="shared" si="0"/>
@@ -13247,7 +13247,7 @@
       </c>
       <c r="BL43" s="7"/>
     </row>
-    <row r="44" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:64" ht="18.75" customHeight="1">
       <c r="B44" t="s">
         <v>1108</v>
       </c>
@@ -13403,7 +13403,7 @@
         <v>[39.781885,-104.891501],</v>
       </c>
     </row>
-    <row r="45" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:64" ht="18.75" customHeight="1">
       <c r="B45" t="s">
         <v>68</v>
       </c>
@@ -13453,7 +13453,7 @@
         <v>421</v>
       </c>
       <c r="V45" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="W45" t="str">
         <f t="shared" si="0"/>
@@ -13603,7 +13603,7 @@
       </c>
       <c r="BL45" s="7"/>
     </row>
-    <row r="46" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:64" ht="18.75" customHeight="1">
       <c r="B46" t="s">
         <v>838</v>
       </c>
@@ -13793,7 +13793,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:64" ht="18.75" customHeight="1">
       <c r="B47" t="s">
         <v>1227</v>
       </c>
@@ -13994,7 +13994,7 @@
         <v>[39.7499044,-104.9997273],</v>
       </c>
     </row>
-    <row r="48" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:64" ht="18.75" customHeight="1">
       <c r="B48" t="s">
         <v>250</v>
       </c>
@@ -14161,7 +14161,7 @@
       </c>
       <c r="BL48" s="7"/>
     </row>
-    <row r="49" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:64" ht="18.75" customHeight="1">
       <c r="B49" t="s">
         <v>252</v>
       </c>
@@ -14325,7 +14325,7 @@
       </c>
       <c r="BL49" s="7"/>
     </row>
-    <row r="50" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:64" ht="18.75" customHeight="1">
       <c r="B50" t="s">
         <v>69</v>
       </c>
@@ -14486,7 +14486,7 @@
       </c>
       <c r="BL50" s="7"/>
     </row>
-    <row r="51" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:64" ht="18.75" customHeight="1">
       <c r="B51" t="s">
         <v>1143</v>
       </c>
@@ -14672,7 +14672,7 @@
         <v>[39.73225,-105.00513],</v>
       </c>
     </row>
-    <row r="52" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:64" ht="18.75" customHeight="1">
       <c r="B52" t="s">
         <v>1160</v>
       </c>
@@ -14716,7 +14716,7 @@
         <v>1900</v>
       </c>
       <c r="V52" s="21" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="W52" t="str">
         <f t="shared" si="0"/>
@@ -14861,7 +14861,7 @@
         <v>[39.7096,-104.98058],</v>
       </c>
     </row>
-    <row r="53" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:64" ht="18.75" customHeight="1">
       <c r="B53" t="s">
         <v>70</v>
       </c>
@@ -14917,7 +14917,7 @@
         <v>421</v>
       </c>
       <c r="V53" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="W53">
         <f t="shared" si="0"/>
@@ -15067,7 +15067,7 @@
       </c>
       <c r="BL53" s="7"/>
     </row>
-    <row r="54" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:64" ht="18.75" customHeight="1">
       <c r="B54" t="s">
         <v>71</v>
       </c>
@@ -15273,7 +15273,7 @@
       </c>
       <c r="BL54" s="7"/>
     </row>
-    <row r="55" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:64" ht="18.75" customHeight="1">
       <c r="B55" t="s">
         <v>832</v>
       </c>
@@ -15466,7 +15466,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:64" ht="18.75" customHeight="1">
       <c r="B56" t="s">
         <v>72</v>
       </c>
@@ -15674,7 +15674,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="57" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:64" ht="18.75" customHeight="1">
       <c r="B57" t="s">
         <v>873</v>
       </c>
@@ -15873,7 +15873,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:64" ht="18.75" customHeight="1">
       <c r="B58" t="s">
         <v>172</v>
       </c>
@@ -16067,7 +16067,7 @@
       </c>
       <c r="BL58" s="7"/>
     </row>
-    <row r="59" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:64" ht="18.75" customHeight="1">
       <c r="B59" t="s">
         <v>263</v>
       </c>
@@ -16231,7 +16231,7 @@
       </c>
       <c r="BL59" s="7"/>
     </row>
-    <row r="60" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:64" ht="18.75" customHeight="1">
       <c r="B60" t="s">
         <v>73</v>
       </c>
@@ -16281,7 +16281,7 @@
         <v>421</v>
       </c>
       <c r="V60" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="W60">
         <f t="shared" si="0"/>
@@ -16431,7 +16431,7 @@
       </c>
       <c r="BL60" s="7"/>
     </row>
-    <row r="61" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:64" ht="18.75" customHeight="1">
       <c r="B61" t="s">
         <v>173</v>
       </c>
@@ -16625,7 +16625,7 @@
       </c>
       <c r="BL61" s="7"/>
     </row>
-    <row r="62" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:64" ht="18.75" customHeight="1">
       <c r="B62" t="s">
         <v>1126</v>
       </c>
@@ -16781,7 +16781,7 @@
         <v>[39.692846,-104.980251],</v>
       </c>
     </row>
-    <row r="63" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:64" ht="18.75" customHeight="1">
       <c r="B63" t="s">
         <v>859</v>
       </c>
@@ -16986,7 +16986,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:64" ht="18.75" customHeight="1">
       <c r="B64" t="s">
         <v>74</v>
       </c>
@@ -17030,7 +17030,7 @@
         <v>422</v>
       </c>
       <c r="V64" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="W64" t="str">
         <f t="shared" si="0"/>
@@ -17180,7 +17180,7 @@
       </c>
       <c r="BL64" s="7"/>
     </row>
-    <row r="65" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:64" ht="18.75" customHeight="1">
       <c r="B65" t="s">
         <v>842</v>
       </c>
@@ -17377,7 +17377,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:64" ht="18.75" customHeight="1">
       <c r="B66" t="s">
         <v>174</v>
       </c>
@@ -17571,7 +17571,7 @@
       </c>
       <c r="BL66" s="7"/>
     </row>
-    <row r="67" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:64" ht="18.75" customHeight="1">
       <c r="B67" t="s">
         <v>75</v>
       </c>
@@ -17777,7 +17777,7 @@
       </c>
       <c r="BL67" s="7"/>
     </row>
-    <row r="68" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:64" ht="18.75" customHeight="1">
       <c r="B68" t="s">
         <v>76</v>
       </c>
@@ -17983,7 +17983,7 @@
       </c>
       <c r="BL68" s="7"/>
     </row>
-    <row r="69" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:64" ht="18.75" customHeight="1">
       <c r="B69" t="s">
         <v>1278</v>
       </c>
@@ -18189,7 +18189,7 @@
       </c>
       <c r="BL69" s="7"/>
     </row>
-    <row r="70" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:64" ht="18.75" customHeight="1">
       <c r="B70" t="s">
         <v>175</v>
       </c>
@@ -18383,7 +18383,7 @@
       </c>
       <c r="BL70" s="7"/>
     </row>
-    <row r="71" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:64" ht="18.75" customHeight="1">
       <c r="B71" t="s">
         <v>176</v>
       </c>
@@ -18580,7 +18580,7 @@
       </c>
       <c r="BL71" s="7"/>
     </row>
-    <row r="72" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:64" ht="18.75" customHeight="1">
       <c r="B72" t="s">
         <v>877</v>
       </c>
@@ -18785,7 +18785,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:64" ht="18.75" customHeight="1">
       <c r="B73" t="s">
         <v>177</v>
       </c>
@@ -18979,7 +18979,7 @@
       </c>
       <c r="BL73" s="7"/>
     </row>
-    <row r="74" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:64" ht="18.75" customHeight="1">
       <c r="B74" t="s">
         <v>247</v>
       </c>
@@ -19188,7 +19188,7 @@
       </c>
       <c r="BL74" s="7"/>
     </row>
-    <row r="75" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:64" ht="18.75" customHeight="1">
       <c r="B75" t="s">
         <v>1234</v>
       </c>
@@ -19384,7 +19384,7 @@
       </c>
       <c r="BL75" s="7"/>
     </row>
-    <row r="76" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:64" ht="18.75" customHeight="1">
       <c r="B76" t="s">
         <v>178</v>
       </c>
@@ -19578,7 +19578,7 @@
       </c>
       <c r="BL76" s="7"/>
     </row>
-    <row r="77" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:64" ht="18.75" customHeight="1">
       <c r="B77" t="s">
         <v>896</v>
       </c>
@@ -19783,7 +19783,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:64" ht="18.75" customHeight="1">
       <c r="B78" t="s">
         <v>844</v>
       </c>
@@ -19976,7 +19976,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:64" ht="18.75" customHeight="1">
       <c r="B79" t="s">
         <v>77</v>
       </c>
@@ -20182,7 +20182,7 @@
       </c>
       <c r="BL79" s="7"/>
     </row>
-    <row r="80" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:64" ht="18.75" customHeight="1">
       <c r="B80" t="s">
         <v>78</v>
       </c>
@@ -20370,7 +20370,7 @@
       </c>
       <c r="BL80" s="7"/>
     </row>
-    <row r="81" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:64" ht="18.75" customHeight="1">
       <c r="B81" t="s">
         <v>241</v>
       </c>
@@ -20537,7 +20537,7 @@
       </c>
       <c r="BL81" s="7"/>
     </row>
-    <row r="82" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:64" ht="18.75" customHeight="1">
       <c r="B82" t="s">
         <v>179</v>
       </c>
@@ -20731,7 +20731,7 @@
       </c>
       <c r="BL82" s="7"/>
     </row>
-    <row r="83" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:64" ht="18.75" customHeight="1">
       <c r="B83" t="s">
         <v>1096</v>
       </c>
@@ -20927,7 +20927,7 @@
       </c>
       <c r="BL83" s="7"/>
     </row>
-    <row r="84" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:64" ht="18.75" customHeight="1">
       <c r="B84" t="s">
         <v>253</v>
       </c>
@@ -21091,7 +21091,7 @@
       </c>
       <c r="BL84" s="7"/>
     </row>
-    <row r="85" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:64" ht="18.75" customHeight="1">
       <c r="B85" t="s">
         <v>180</v>
       </c>
@@ -21285,7 +21285,7 @@
       </c>
       <c r="BL85" s="7"/>
     </row>
-    <row r="86" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:64" ht="18.75" customHeight="1">
       <c r="B86" t="s">
         <v>181</v>
       </c>
@@ -21479,7 +21479,7 @@
       </c>
       <c r="BL86" s="7"/>
     </row>
-    <row r="87" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:64" ht="18.75" customHeight="1">
       <c r="B87" t="s">
         <v>1246</v>
       </c>
@@ -21681,7 +21681,7 @@
       </c>
       <c r="BL87" s="7"/>
     </row>
-    <row r="88" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:64" ht="18.75" customHeight="1">
       <c r="B88" t="s">
         <v>1109</v>
       </c>
@@ -21837,7 +21837,7 @@
         <v>[39.694056,-104.987055],</v>
       </c>
     </row>
-    <row r="89" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:64" ht="18.75" customHeight="1">
       <c r="B89" t="s">
         <v>182</v>
       </c>
@@ -22031,7 +22031,7 @@
       </c>
       <c r="BL89" s="7"/>
     </row>
-    <row r="90" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:64" ht="18.75" customHeight="1">
       <c r="B90" t="s">
         <v>183</v>
       </c>
@@ -22225,7 +22225,7 @@
       </c>
       <c r="BL90" s="7"/>
     </row>
-    <row r="91" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:64" ht="18.75" customHeight="1">
       <c r="B91" t="s">
         <v>249</v>
       </c>
@@ -22437,7 +22437,7 @@
       </c>
       <c r="BL91" s="7"/>
     </row>
-    <row r="92" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:64" ht="18.75" customHeight="1">
       <c r="B92" t="s">
         <v>1162</v>
       </c>
@@ -22638,7 +22638,7 @@
         <v>[39.76211,-105.01623],</v>
       </c>
     </row>
-    <row r="93" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:64" ht="18.75" customHeight="1">
       <c r="B93" t="s">
         <v>79</v>
       </c>
@@ -22847,7 +22847,7 @@
       </c>
       <c r="BL93" s="7"/>
     </row>
-    <row r="94" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:64" ht="18.75" customHeight="1">
       <c r="B94" t="s">
         <v>184</v>
       </c>
@@ -23041,7 +23041,7 @@
       </c>
       <c r="BL94" s="7"/>
     </row>
-    <row r="95" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:64" ht="18.75" customHeight="1">
       <c r="B95" t="s">
         <v>58</v>
       </c>
@@ -23247,7 +23247,7 @@
       </c>
       <c r="BL95" s="7"/>
     </row>
-    <row r="96" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:64" ht="18.75" customHeight="1">
       <c r="B96" t="s">
         <v>80</v>
       </c>
@@ -23441,7 +23441,7 @@
       </c>
       <c r="BL96" s="7"/>
     </row>
-    <row r="97" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:64" ht="18.75" customHeight="1">
       <c r="B97" t="s">
         <v>81</v>
       </c>
@@ -23650,7 +23650,7 @@
       </c>
       <c r="BL97" s="7"/>
     </row>
-    <row r="98" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:64" ht="18.75" customHeight="1">
       <c r="B98" t="s">
         <v>934</v>
       </c>
@@ -23843,7 +23843,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:64" ht="18.75" customHeight="1">
       <c r="B99" t="s">
         <v>863</v>
       </c>
@@ -24048,7 +24048,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:64" ht="18.75" customHeight="1">
       <c r="B100" t="s">
         <v>82</v>
       </c>
@@ -24254,7 +24254,7 @@
       </c>
       <c r="BL100" s="7"/>
     </row>
-    <row r="101" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:64" ht="18.75" customHeight="1">
       <c r="B101" t="s">
         <v>265</v>
       </c>
@@ -24430,7 +24430,7 @@
       </c>
       <c r="BL101" s="7"/>
     </row>
-    <row r="102" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:64" ht="18.75" customHeight="1">
       <c r="B102" t="s">
         <v>83</v>
       </c>
@@ -24636,7 +24636,7 @@
       </c>
       <c r="BL102" s="7"/>
     </row>
-    <row r="103" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:64" ht="18.75" customHeight="1">
       <c r="B103" t="s">
         <v>255</v>
       </c>
@@ -24800,7 +24800,7 @@
       </c>
       <c r="BL103" s="7"/>
     </row>
-    <row r="104" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:64" ht="18.75" customHeight="1">
       <c r="B104" t="s">
         <v>84</v>
       </c>
@@ -25009,7 +25009,7 @@
       </c>
       <c r="BL104" s="7"/>
     </row>
-    <row r="105" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:64" ht="18.75" customHeight="1">
       <c r="B105" t="s">
         <v>894</v>
       </c>
@@ -25169,7 +25169,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:64" ht="18.75" customHeight="1">
       <c r="B106" t="s">
         <v>854</v>
       </c>
@@ -25329,7 +25329,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:64" ht="18.75" customHeight="1">
       <c r="B107" t="s">
         <v>85</v>
       </c>
@@ -25541,7 +25541,7 @@
       </c>
       <c r="BL107" s="7"/>
     </row>
-    <row r="108" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:64" ht="18.75" customHeight="1">
       <c r="B108" t="s">
         <v>185</v>
       </c>
@@ -25729,7 +25729,7 @@
       </c>
       <c r="BL108" s="7"/>
     </row>
-    <row r="109" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:64" ht="18.75" customHeight="1">
       <c r="B109" t="s">
         <v>86</v>
       </c>
@@ -25935,7 +25935,7 @@
       </c>
       <c r="BL109" s="7"/>
     </row>
-    <row r="110" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:64" ht="18.75" customHeight="1">
       <c r="B110" t="s">
         <v>186</v>
       </c>
@@ -26129,7 +26129,7 @@
       </c>
       <c r="BL110" s="7"/>
     </row>
-    <row r="111" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:64" ht="18.75" customHeight="1">
       <c r="B111" t="s">
         <v>87</v>
       </c>
@@ -26290,7 +26290,7 @@
       </c>
       <c r="BL111" s="7"/>
     </row>
-    <row r="112" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:64" ht="18.75" customHeight="1">
       <c r="B112" t="s">
         <v>245</v>
       </c>
@@ -26499,7 +26499,7 @@
       </c>
       <c r="BL112" s="7"/>
     </row>
-    <row r="113" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:64" ht="18.75" customHeight="1">
       <c r="B113" t="s">
         <v>88</v>
       </c>
@@ -26660,7 +26660,7 @@
       </c>
       <c r="BL113" s="7"/>
     </row>
-    <row r="114" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:64" ht="18.75" customHeight="1">
       <c r="B114" t="s">
         <v>883</v>
       </c>
@@ -26859,7 +26859,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:64" ht="18.75" customHeight="1">
       <c r="B115" t="s">
         <v>89</v>
       </c>
@@ -27065,7 +27065,7 @@
       </c>
       <c r="BL115" s="7"/>
     </row>
-    <row r="116" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:64" ht="18.75" customHeight="1">
       <c r="B116" t="s">
         <v>90</v>
       </c>
@@ -27268,7 +27268,7 @@
       </c>
       <c r="BL116" s="7"/>
     </row>
-    <row r="117" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:64" ht="18.75" customHeight="1">
       <c r="B117" t="s">
         <v>922</v>
       </c>
@@ -27473,7 +27473,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:64" ht="18.75" customHeight="1">
       <c r="B118" t="s">
         <v>187</v>
       </c>
@@ -27667,7 +27667,7 @@
       </c>
       <c r="BL118" s="7"/>
     </row>
-    <row r="119" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:64" ht="18.75" customHeight="1">
       <c r="B119" t="s">
         <v>232</v>
       </c>
@@ -27852,7 +27852,7 @@
       </c>
       <c r="BL119" s="7"/>
     </row>
-    <row r="120" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:64" ht="18.75" customHeight="1">
       <c r="B120" t="s">
         <v>188</v>
       </c>
@@ -28047,7 +28047,7 @@
       </c>
       <c r="BL120" s="7"/>
     </row>
-    <row r="121" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:64" ht="18.75" customHeight="1">
       <c r="B121" t="s">
         <v>91</v>
       </c>
@@ -28241,7 +28241,7 @@
       </c>
       <c r="BL121" s="7"/>
     </row>
-    <row r="122" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:64" ht="18.75" customHeight="1">
       <c r="B122" t="s">
         <v>92</v>
       </c>
@@ -28438,7 +28438,7 @@
       </c>
       <c r="BL122" s="7"/>
     </row>
-    <row r="123" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:64" ht="18.75" customHeight="1">
       <c r="B123" t="s">
         <v>93</v>
       </c>
@@ -28647,7 +28647,7 @@
       </c>
       <c r="BL123" s="7"/>
     </row>
-    <row r="124" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:64" ht="18.75" customHeight="1">
       <c r="B124" t="s">
         <v>240</v>
       </c>
@@ -28844,7 +28844,7 @@
       </c>
       <c r="BL124" s="7"/>
     </row>
-    <row r="125" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:64" ht="18.75" customHeight="1">
       <c r="B125" t="s">
         <v>189</v>
       </c>
@@ -29044,7 +29044,7 @@
       </c>
       <c r="BL125" s="7"/>
     </row>
-    <row r="126" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:64" ht="18.75" customHeight="1">
       <c r="B126" t="s">
         <v>190</v>
       </c>
@@ -29238,7 +29238,7 @@
       </c>
       <c r="BL126" s="7"/>
     </row>
-    <row r="127" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:64" ht="18.75" customHeight="1">
       <c r="B127" t="s">
         <v>94</v>
       </c>
@@ -29444,7 +29444,7 @@
       </c>
       <c r="BL127" s="7"/>
     </row>
-    <row r="128" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:64" ht="18.75" customHeight="1">
       <c r="B128" t="s">
         <v>898</v>
       </c>
@@ -29604,7 +29604,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:64" ht="18.75" customHeight="1">
       <c r="B129" t="s">
         <v>95</v>
       </c>
@@ -29814,7 +29814,7 @@
       </c>
       <c r="BL129" s="7"/>
     </row>
-    <row r="130" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:64" ht="18.75" customHeight="1">
       <c r="B130" t="s">
         <v>96</v>
       </c>
@@ -30008,7 +30008,7 @@
       </c>
       <c r="BL130" s="7"/>
     </row>
-    <row r="131" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:64" ht="18.75" customHeight="1">
       <c r="B131" t="s">
         <v>1135</v>
       </c>
@@ -30209,7 +30209,7 @@
         <v>[39.75576,-104.99021],</v>
       </c>
     </row>
-    <row r="132" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:64" ht="18.75" customHeight="1">
       <c r="B132" t="s">
         <v>97</v>
       </c>
@@ -30418,7 +30418,7 @@
       </c>
       <c r="BL132" s="7"/>
     </row>
-    <row r="133" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:64" ht="18.75" customHeight="1">
       <c r="B133" s="1" t="s">
         <v>852</v>
       </c>
@@ -30578,7 +30578,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:64" ht="18.75" customHeight="1">
       <c r="B134" t="s">
         <v>98</v>
       </c>
@@ -30784,7 +30784,7 @@
       </c>
       <c r="BL134" s="7"/>
     </row>
-    <row r="135" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:64" ht="18.75" customHeight="1">
       <c r="B135" t="s">
         <v>99</v>
       </c>
@@ -30978,7 +30978,7 @@
       </c>
       <c r="BL135" s="7"/>
     </row>
-    <row r="136" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:64" ht="18.75" customHeight="1">
       <c r="B136" t="s">
         <v>100</v>
       </c>
@@ -31187,7 +31187,7 @@
       </c>
       <c r="BL136" s="7"/>
     </row>
-    <row r="137" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:64" ht="18.75" customHeight="1">
       <c r="B137" t="s">
         <v>1242</v>
       </c>
@@ -31377,7 +31377,7 @@
       </c>
       <c r="BL137" s="7"/>
     </row>
-    <row r="138" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:64" ht="18.75" customHeight="1">
       <c r="B138" t="s">
         <v>233</v>
       </c>
@@ -31574,7 +31574,7 @@
       </c>
       <c r="BL138" s="7"/>
     </row>
-    <row r="139" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:64" ht="18.75" customHeight="1">
       <c r="B139" t="s">
         <v>101</v>
       </c>
@@ -31738,7 +31738,7 @@
       </c>
       <c r="BL139" s="7"/>
     </row>
-    <row r="140" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:64" ht="18.75" customHeight="1">
       <c r="B140" s="9" t="s">
         <v>102</v>
       </c>
@@ -31947,7 +31947,7 @@
       </c>
       <c r="BL140" s="7"/>
     </row>
-    <row r="141" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:64" ht="18.75" customHeight="1">
       <c r="B141" t="s">
         <v>103</v>
       </c>
@@ -32153,7 +32153,7 @@
       </c>
       <c r="BL141" s="7"/>
     </row>
-    <row r="142" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:64" ht="18.75" customHeight="1">
       <c r="B142" t="s">
         <v>104</v>
       </c>
@@ -32359,7 +32359,7 @@
       </c>
       <c r="BL142" s="7"/>
     </row>
-    <row r="143" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:64" ht="18.75" customHeight="1">
       <c r="B143" t="s">
         <v>1154</v>
       </c>
@@ -32560,7 +32560,7 @@
         <v>[39.75382,-104.99643],</v>
       </c>
     </row>
-    <row r="144" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:64" ht="18.75" customHeight="1">
       <c r="B144" t="s">
         <v>105</v>
       </c>
@@ -32766,7 +32766,7 @@
       </c>
       <c r="BL144" s="7"/>
     </row>
-    <row r="145" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:64" ht="18.75" customHeight="1">
       <c r="B145" t="s">
         <v>1263</v>
       </c>
@@ -32964,7 +32964,7 @@
         <v>[39.76944,-104.97676],</v>
       </c>
     </row>
-    <row r="146" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:64" ht="18.75" customHeight="1">
       <c r="B146" t="s">
         <v>191</v>
       </c>
@@ -33140,7 +33140,7 @@
       </c>
       <c r="BL146" s="7"/>
     </row>
-    <row r="147" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:64" ht="18.75" customHeight="1">
       <c r="B147" t="s">
         <v>106</v>
       </c>
@@ -33334,7 +33334,7 @@
       </c>
       <c r="BL147" s="7"/>
     </row>
-    <row r="148" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:64" ht="18.75" customHeight="1">
       <c r="B148" t="s">
         <v>107</v>
       </c>
@@ -33540,7 +33540,7 @@
       </c>
       <c r="BL148" s="7"/>
     </row>
-    <row r="149" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:64" ht="18.75" customHeight="1">
       <c r="B149" t="s">
         <v>908</v>
       </c>
@@ -33739,7 +33739,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:64" ht="18.75" customHeight="1">
       <c r="B150" t="s">
         <v>828</v>
       </c>
@@ -33938,7 +33938,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:64" ht="18.75" customHeight="1">
       <c r="B151" t="s">
         <v>848</v>
       </c>
@@ -34143,7 +34143,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:64" ht="18.75" customHeight="1">
       <c r="B152" t="s">
         <v>1230</v>
       </c>
@@ -34338,7 +34338,7 @@
         <v>[39.7505999,-104.9994734],</v>
       </c>
     </row>
-    <row r="153" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:64" ht="18.75" customHeight="1">
       <c r="B153" t="s">
         <v>108</v>
       </c>
@@ -34544,7 +34544,7 @@
       </c>
       <c r="BL153" s="7"/>
     </row>
-    <row r="154" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:64" ht="18.75" customHeight="1">
       <c r="B154" t="s">
         <v>192</v>
       </c>
@@ -34735,7 +34735,7 @@
       </c>
       <c r="BL154" s="7"/>
     </row>
-    <row r="155" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:64" ht="18.75" customHeight="1">
       <c r="B155" t="s">
         <v>193</v>
       </c>
@@ -34932,7 +34932,7 @@
       </c>
       <c r="BL155" s="7"/>
     </row>
-    <row r="156" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:64" ht="18.75" customHeight="1">
       <c r="B156" t="s">
         <v>109</v>
       </c>
@@ -35132,7 +35132,7 @@
       </c>
       <c r="BL156" s="7"/>
     </row>
-    <row r="157" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:64" ht="18.75" customHeight="1">
       <c r="B157" t="s">
         <v>194</v>
       </c>
@@ -35329,7 +35329,7 @@
       </c>
       <c r="BL157" s="7"/>
     </row>
-    <row r="158" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:64" ht="18.75" customHeight="1">
       <c r="B158" t="s">
         <v>110</v>
       </c>
@@ -35526,7 +35526,7 @@
       </c>
       <c r="BL158" s="7"/>
     </row>
-    <row r="159" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:64" ht="18.75" customHeight="1">
       <c r="B159" t="s">
         <v>111</v>
       </c>
@@ -35720,7 +35720,7 @@
       </c>
       <c r="BL159" s="7"/>
     </row>
-    <row r="160" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:64" ht="18.75" customHeight="1">
       <c r="B160" t="s">
         <v>112</v>
       </c>
@@ -35914,7 +35914,7 @@
       </c>
       <c r="BL160" s="7"/>
     </row>
-    <row r="161" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:64" ht="18.75" customHeight="1">
       <c r="B161" t="s">
         <v>113</v>
       </c>
@@ -36114,7 +36114,7 @@
       </c>
       <c r="BL161" s="7"/>
     </row>
-    <row r="162" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:64" ht="18.75" customHeight="1">
       <c r="B162" t="s">
         <v>195</v>
       </c>
@@ -36311,7 +36311,7 @@
       </c>
       <c r="BL162" s="7"/>
     </row>
-    <row r="163" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:64" ht="18.75" customHeight="1">
       <c r="B163" t="s">
         <v>196</v>
       </c>
@@ -36505,7 +36505,7 @@
       </c>
       <c r="BL163" s="7"/>
     </row>
-    <row r="164" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:64" ht="18.75" customHeight="1">
       <c r="B164" t="s">
         <v>972</v>
       </c>
@@ -36698,7 +36698,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:64" ht="18.75" customHeight="1">
       <c r="B165" t="s">
         <v>114</v>
       </c>
@@ -36904,7 +36904,7 @@
       </c>
       <c r="BL165" s="7"/>
     </row>
-    <row r="166" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:64" ht="18.75" customHeight="1">
       <c r="B166" t="s">
         <v>197</v>
       </c>
@@ -37098,7 +37098,7 @@
       </c>
       <c r="BL166" s="7"/>
     </row>
-    <row r="167" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:64" ht="18.75" customHeight="1">
       <c r="B167" t="s">
         <v>198</v>
       </c>
@@ -37292,7 +37292,7 @@
       </c>
       <c r="BL167" s="7"/>
     </row>
-    <row r="168" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:64" ht="18.75" customHeight="1">
       <c r="B168" t="s">
         <v>115</v>
       </c>
@@ -37498,7 +37498,7 @@
       </c>
       <c r="BL168" s="7"/>
     </row>
-    <row r="169" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:64" ht="18.75" customHeight="1">
       <c r="B169" t="s">
         <v>116</v>
       </c>
@@ -37704,7 +37704,7 @@
       </c>
       <c r="BL169" s="7"/>
     </row>
-    <row r="170" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:64" ht="18.75" customHeight="1">
       <c r="B170" t="s">
         <v>117</v>
       </c>
@@ -37910,7 +37910,7 @@
       </c>
       <c r="BL170" s="7"/>
     </row>
-    <row r="171" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:64" ht="18.75" customHeight="1">
       <c r="B171" t="s">
         <v>118</v>
       </c>
@@ -38116,7 +38116,7 @@
       </c>
       <c r="BL171" s="7"/>
     </row>
-    <row r="172" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:64" ht="18.75" customHeight="1">
       <c r="B172" t="s">
         <v>119</v>
       </c>
@@ -38322,7 +38322,7 @@
       </c>
       <c r="BL172" s="7"/>
     </row>
-    <row r="173" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:64" ht="18.75" customHeight="1">
       <c r="B173" t="s">
         <v>120</v>
       </c>
@@ -38516,7 +38516,7 @@
       </c>
       <c r="BL173" s="7"/>
     </row>
-    <row r="174" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:64" ht="18.75" customHeight="1">
       <c r="B174" t="s">
         <v>199</v>
       </c>
@@ -38710,7 +38710,7 @@
       </c>
       <c r="BL174" s="7"/>
     </row>
-    <row r="175" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:64" ht="18.75" customHeight="1">
       <c r="B175" t="s">
         <v>258</v>
       </c>
@@ -38919,7 +38919,7 @@
       </c>
       <c r="BL175" s="7"/>
     </row>
-    <row r="176" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:64" ht="18.75" customHeight="1">
       <c r="B176" t="s">
         <v>121</v>
       </c>
@@ -39125,7 +39125,7 @@
       </c>
       <c r="BL176" s="7"/>
     </row>
-    <row r="177" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:64" ht="18.75" customHeight="1">
       <c r="B177" t="s">
         <v>200</v>
       </c>
@@ -39319,7 +39319,7 @@
       </c>
       <c r="BL177" s="7"/>
     </row>
-    <row r="178" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:64" ht="18.75" customHeight="1">
       <c r="B178" t="s">
         <v>122</v>
       </c>
@@ -39525,7 +39525,7 @@
       </c>
       <c r="BL178" s="7"/>
     </row>
-    <row r="179" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:64" ht="18.75" customHeight="1">
       <c r="B179" t="s">
         <v>201</v>
       </c>
@@ -39719,7 +39719,7 @@
       </c>
       <c r="BL179" s="7"/>
     </row>
-    <row r="180" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:64" ht="18.75" customHeight="1">
       <c r="B180" t="s">
         <v>123</v>
       </c>
@@ -39925,7 +39925,7 @@
       </c>
       <c r="BL180" s="7"/>
     </row>
-    <row r="181" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:64" ht="18.75" customHeight="1">
       <c r="B181" t="s">
         <v>259</v>
       </c>
@@ -40122,7 +40122,7 @@
       </c>
       <c r="BL181" s="7"/>
     </row>
-    <row r="182" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:64" ht="18.75" customHeight="1">
       <c r="B182" s="1" t="s">
         <v>861</v>
       </c>
@@ -40309,7 +40309,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:64" ht="18.75" customHeight="1">
       <c r="B183" t="s">
         <v>869</v>
       </c>
@@ -40514,7 +40514,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:64" ht="18.75" customHeight="1">
       <c r="B184" t="s">
         <v>124</v>
       </c>
@@ -40720,7 +40720,7 @@
       </c>
       <c r="BL184" s="7"/>
     </row>
-    <row r="185" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:64" ht="18.75" customHeight="1">
       <c r="B185" t="s">
         <v>234</v>
       </c>
@@ -40914,7 +40914,7 @@
       </c>
       <c r="BL185" s="7"/>
     </row>
-    <row r="186" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:64" ht="18.75" customHeight="1">
       <c r="B186" t="s">
         <v>264</v>
       </c>
@@ -41099,7 +41099,7 @@
       </c>
       <c r="BL186" s="7"/>
     </row>
-    <row r="187" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:64" ht="18.75" customHeight="1">
       <c r="B187" t="s">
         <v>940</v>
       </c>
@@ -41304,7 +41304,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:64" ht="18.75" customHeight="1">
       <c r="B188" t="s">
         <v>875</v>
       </c>
@@ -41461,7 +41461,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:64" ht="18.75" customHeight="1">
       <c r="B189" t="s">
         <v>202</v>
       </c>
@@ -41661,7 +41661,7 @@
       </c>
       <c r="BL189" s="7"/>
     </row>
-    <row r="190" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:64" ht="18.75" customHeight="1">
       <c r="B190" t="s">
         <v>1110</v>
       </c>
@@ -41817,7 +41817,7 @@
         <v>[39.677478,-104.914182],</v>
       </c>
     </row>
-    <row r="191" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:64" ht="18.75" customHeight="1">
       <c r="B191" t="s">
         <v>856</v>
       </c>
@@ -42022,7 +42022,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:64" ht="18.75" customHeight="1">
       <c r="B192" t="s">
         <v>203</v>
       </c>
@@ -42216,7 +42216,7 @@
       </c>
       <c r="BL192" s="7"/>
     </row>
-    <row r="193" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:64" ht="18.75" customHeight="1">
       <c r="B193" s="6" t="s">
         <v>204</v>
       </c>
@@ -42414,7 +42414,7 @@
       </c>
       <c r="BL193" s="7"/>
     </row>
-    <row r="194" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:64" ht="18.75" customHeight="1">
       <c r="B194" t="s">
         <v>205</v>
       </c>
@@ -42608,7 +42608,7 @@
       </c>
       <c r="BL194" s="7"/>
     </row>
-    <row r="195" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:64" ht="18.75" customHeight="1">
       <c r="B195" t="s">
         <v>206</v>
       </c>
@@ -42802,7 +42802,7 @@
       </c>
       <c r="BL195" s="7"/>
     </row>
-    <row r="196" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:64" ht="18.75" customHeight="1">
       <c r="B196" t="s">
         <v>1176</v>
       </c>
@@ -42985,7 +42985,7 @@
         <v>[39.76354,-105.01106],</v>
       </c>
     </row>
-    <row r="197" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:64" ht="18.75" customHeight="1">
       <c r="B197" t="s">
         <v>1187</v>
       </c>
@@ -43186,7 +43186,7 @@
         <v>[39.71761,-104.94761],</v>
       </c>
     </row>
-    <row r="198" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:64" ht="18.75" customHeight="1">
       <c r="B198" t="s">
         <v>207</v>
       </c>
@@ -43380,7 +43380,7 @@
       </c>
       <c r="BL198" s="7"/>
     </row>
-    <row r="199" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:64" ht="18.75" customHeight="1">
       <c r="B199" t="s">
         <v>1165</v>
       </c>
@@ -43569,7 +43569,7 @@
         <v>[39.74819,-104.99897],</v>
       </c>
     </row>
-    <row r="200" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:64" ht="18.75" customHeight="1">
       <c r="B200" t="s">
         <v>125</v>
       </c>
@@ -43763,7 +43763,7 @@
       </c>
       <c r="BL200" s="7"/>
     </row>
-    <row r="201" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:64" ht="18.75" customHeight="1">
       <c r="B201" t="s">
         <v>900</v>
       </c>
@@ -43956,7 +43956,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:64" ht="18.75" customHeight="1">
       <c r="B202" t="s">
         <v>1168</v>
       </c>
@@ -44145,7 +44145,7 @@
         <v>[39.75959,-104.98604],</v>
       </c>
     </row>
-    <row r="203" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:64" ht="18.75" customHeight="1">
       <c r="B203" t="s">
         <v>126</v>
       </c>
@@ -44345,7 +44345,7 @@
       </c>
       <c r="BL203" s="7"/>
     </row>
-    <row r="204" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:64" ht="18.75" customHeight="1">
       <c r="B204" t="s">
         <v>826</v>
       </c>
@@ -44535,7 +44535,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:64" ht="18.75" customHeight="1">
       <c r="B205" t="s">
         <v>127</v>
       </c>
@@ -44735,7 +44735,7 @@
       </c>
       <c r="BL205" s="7"/>
     </row>
-    <row r="206" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:64" ht="18.75" customHeight="1">
       <c r="B206" t="s">
         <v>128</v>
       </c>
@@ -44941,7 +44941,7 @@
       </c>
       <c r="BL206" s="7"/>
     </row>
-    <row r="207" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:64" ht="18.75" customHeight="1">
       <c r="B207" t="s">
         <v>1132</v>
       </c>
@@ -45131,7 +45131,7 @@
       </c>
       <c r="BL207" s="7"/>
     </row>
-    <row r="208" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:64" ht="18.75" customHeight="1">
       <c r="B208" t="s">
         <v>237</v>
       </c>
@@ -45322,7 +45322,7 @@
       </c>
       <c r="BL208" s="7"/>
     </row>
-    <row r="209" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:64" ht="18.75" customHeight="1">
       <c r="B209" t="s">
         <v>129</v>
       </c>
@@ -45531,7 +45531,7 @@
       </c>
       <c r="BL209" s="7"/>
     </row>
-    <row r="210" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:64" ht="18.75" customHeight="1">
       <c r="B210" t="s">
         <v>130</v>
       </c>
@@ -45725,7 +45725,7 @@
       </c>
       <c r="BL210" s="7"/>
     </row>
-    <row r="211" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:64" ht="18.75" customHeight="1">
       <c r="B211" t="s">
         <v>208</v>
       </c>
@@ -45919,7 +45919,7 @@
       </c>
       <c r="BL211" s="7"/>
     </row>
-    <row r="212" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:64" ht="18.75" customHeight="1">
       <c r="B212" t="s">
         <v>261</v>
       </c>
@@ -46083,7 +46083,7 @@
       </c>
       <c r="BL212" s="7"/>
     </row>
-    <row r="213" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:64" ht="18.75" customHeight="1">
       <c r="B213" t="s">
         <v>131</v>
       </c>
@@ -46277,7 +46277,7 @@
       </c>
       <c r="BL213" s="7"/>
     </row>
-    <row r="214" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:64" ht="18.75" customHeight="1">
       <c r="B214" t="s">
         <v>132</v>
       </c>
@@ -46483,7 +46483,7 @@
       </c>
       <c r="BL214" s="7"/>
     </row>
-    <row r="215" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:64" ht="18.75" customHeight="1">
       <c r="B215" t="s">
         <v>871</v>
       </c>
@@ -46688,7 +46688,7 @@
         <v/>
       </c>
     </row>
-    <row r="216" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:64" ht="18.75" customHeight="1">
       <c r="B216" t="s">
         <v>133</v>
       </c>
@@ -46894,7 +46894,7 @@
       </c>
       <c r="BL216" s="7"/>
     </row>
-    <row r="217" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:64" ht="18.75" customHeight="1">
       <c r="B217" t="s">
         <v>251</v>
       </c>
@@ -47094,7 +47094,7 @@
       </c>
       <c r="BL217" s="7"/>
     </row>
-    <row r="218" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:64" ht="18.75" customHeight="1">
       <c r="B218" t="s">
         <v>936</v>
       </c>
@@ -47254,7 +47254,7 @@
         <v/>
       </c>
     </row>
-    <row r="219" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:64" ht="18.75" customHeight="1">
       <c r="B219" t="s">
         <v>260</v>
       </c>
@@ -47418,7 +47418,7 @@
       </c>
       <c r="BL219" s="7"/>
     </row>
-    <row r="220" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:64" ht="18.75" customHeight="1">
       <c r="B220" t="s">
         <v>242</v>
       </c>
@@ -47616,7 +47616,7 @@
       </c>
       <c r="BL220" s="7"/>
     </row>
-    <row r="221" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:64" ht="18.75" customHeight="1">
       <c r="B221" t="s">
         <v>134</v>
       </c>
@@ -47816,7 +47816,7 @@
       </c>
       <c r="BL221" s="7"/>
     </row>
-    <row r="222" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:64" ht="18.75" customHeight="1">
       <c r="B222" t="s">
         <v>135</v>
       </c>
@@ -48022,7 +48022,7 @@
       </c>
       <c r="BL222" s="7"/>
     </row>
-    <row r="223" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:64" ht="18.75" customHeight="1">
       <c r="B223" t="s">
         <v>209</v>
       </c>
@@ -48216,7 +48216,7 @@
       </c>
       <c r="BL223" s="7"/>
     </row>
-    <row r="224" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:64" ht="18.75" customHeight="1">
       <c r="B224" t="s">
         <v>136</v>
       </c>
@@ -48422,7 +48422,7 @@
       </c>
       <c r="BL224" s="7"/>
     </row>
-    <row r="225" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:64" ht="18.75" customHeight="1">
       <c r="B225" t="s">
         <v>904</v>
       </c>
@@ -48582,7 +48582,7 @@
         <v/>
       </c>
     </row>
-    <row r="226" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:64" ht="18.75" customHeight="1">
       <c r="B226" t="s">
         <v>137</v>
       </c>
@@ -48776,7 +48776,7 @@
       </c>
       <c r="BL226" s="7"/>
     </row>
-    <row r="227" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:64" ht="18.75" customHeight="1">
       <c r="B227" t="s">
         <v>138</v>
       </c>
@@ -48982,7 +48982,7 @@
       </c>
       <c r="BL227" s="7"/>
     </row>
-    <row r="228" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:64" ht="18.75" customHeight="1">
       <c r="B228" t="s">
         <v>139</v>
       </c>
@@ -49188,7 +49188,7 @@
       </c>
       <c r="BL228" s="7"/>
     </row>
-    <row r="229" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:64" ht="18.75" customHeight="1">
       <c r="B229" t="s">
         <v>262</v>
       </c>
@@ -49352,7 +49352,7 @@
       </c>
       <c r="BL229" s="7"/>
     </row>
-    <row r="230" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:64" ht="18.75" customHeight="1">
       <c r="B230" t="s">
         <v>1239</v>
       </c>
@@ -49539,7 +49539,7 @@
       </c>
       <c r="BL230" s="7"/>
     </row>
-    <row r="231" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:64" ht="18.75" customHeight="1">
       <c r="B231" t="s">
         <v>140</v>
       </c>
@@ -49736,7 +49736,7 @@
       </c>
       <c r="BL231" s="7"/>
     </row>
-    <row r="232" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:64" ht="18.75" customHeight="1">
       <c r="B232" t="s">
         <v>840</v>
       </c>
@@ -49941,7 +49941,7 @@
         <v/>
       </c>
     </row>
-    <row r="233" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:64" ht="18.75" customHeight="1">
       <c r="B233" t="s">
         <v>210</v>
       </c>
@@ -50135,7 +50135,7 @@
       </c>
       <c r="BL233" s="7"/>
     </row>
-    <row r="234" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:64" ht="18.75" customHeight="1">
       <c r="B234" t="s">
         <v>916</v>
       </c>
@@ -50295,7 +50295,7 @@
         <v/>
       </c>
     </row>
-    <row r="235" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:64" ht="18.75" customHeight="1">
       <c r="B235" t="s">
         <v>1111</v>
       </c>
@@ -50496,7 +50496,7 @@
         <v>[39.753306,-104.996116],</v>
       </c>
     </row>
-    <row r="236" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:64" ht="18.75" customHeight="1">
       <c r="B236" t="s">
         <v>211</v>
       </c>
@@ -50693,7 +50693,7 @@
       </c>
       <c r="BL236" s="7"/>
     </row>
-    <row r="237" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:64" ht="18.75" customHeight="1">
       <c r="B237" t="s">
         <v>141</v>
       </c>
@@ -50893,7 +50893,7 @@
       </c>
       <c r="BL237" s="7"/>
     </row>
-    <row r="238" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:64" ht="18.75" customHeight="1">
       <c r="B238" t="s">
         <v>1100</v>
       </c>
@@ -51050,7 +51050,7 @@
       </c>
       <c r="BL238" s="7"/>
     </row>
-    <row r="239" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:64" ht="18.75" customHeight="1">
       <c r="B239" t="s">
         <v>890</v>
       </c>
@@ -51255,7 +51255,7 @@
         <v/>
       </c>
     </row>
-    <row r="240" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:64" ht="18.75" customHeight="1">
       <c r="B240" t="s">
         <v>142</v>
       </c>
@@ -51461,7 +51461,7 @@
       </c>
       <c r="BL240" s="7"/>
     </row>
-    <row r="241" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:64" ht="18.75" customHeight="1">
       <c r="B241" t="s">
         <v>906</v>
       </c>
@@ -51618,7 +51618,7 @@
         <v/>
       </c>
     </row>
-    <row r="242" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:64" ht="18.75" customHeight="1">
       <c r="B242" t="s">
         <v>878</v>
       </c>
@@ -51824,7 +51824,7 @@
       </c>
       <c r="BL242" s="7"/>
     </row>
-    <row r="243" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:64" ht="18.75" customHeight="1">
       <c r="B243" t="s">
         <v>212</v>
       </c>
@@ -52018,7 +52018,7 @@
       </c>
       <c r="BL243" s="7"/>
     </row>
-    <row r="244" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:64" ht="18.75" customHeight="1">
       <c r="B244" t="s">
         <v>213</v>
       </c>
@@ -52212,7 +52212,7 @@
       </c>
       <c r="BL244" s="7"/>
     </row>
-    <row r="245" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:64" ht="18.75" customHeight="1">
       <c r="B245" t="s">
         <v>214</v>
       </c>
@@ -52406,7 +52406,7 @@
       </c>
       <c r="BL245" s="7"/>
     </row>
-    <row r="246" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:64" ht="18.75" customHeight="1">
       <c r="B246" t="s">
         <v>1254</v>
       </c>
@@ -52596,7 +52596,7 @@
       </c>
       <c r="BL246" s="7"/>
     </row>
-    <row r="247" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:64" ht="18.75" customHeight="1">
       <c r="B247" t="s">
         <v>215</v>
       </c>
@@ -52790,7 +52790,7 @@
       </c>
       <c r="BL247" s="7"/>
     </row>
-    <row r="248" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:64" ht="18.75" customHeight="1">
       <c r="B248" t="s">
         <v>143</v>
       </c>
@@ -52996,7 +52996,7 @@
       </c>
       <c r="BL248" s="7"/>
     </row>
-    <row r="249" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:64" ht="18.75" customHeight="1">
       <c r="B249" t="s">
         <v>256</v>
       </c>
@@ -53160,7 +53160,7 @@
       </c>
       <c r="BL249" s="7"/>
     </row>
-    <row r="250" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:64" ht="18.75" customHeight="1">
       <c r="B250" t="s">
         <v>243</v>
       </c>
@@ -53324,7 +53324,7 @@
       </c>
       <c r="BL250" s="7"/>
     </row>
-    <row r="251" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:64" ht="18.75" customHeight="1">
       <c r="B251" t="s">
         <v>144</v>
       </c>
@@ -53530,7 +53530,7 @@
       </c>
       <c r="BL251" s="7"/>
     </row>
-    <row r="252" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:64" ht="18.75" customHeight="1">
       <c r="B252" t="s">
         <v>216</v>
       </c>
@@ -53724,7 +53724,7 @@
       </c>
       <c r="BL252" s="7"/>
     </row>
-    <row r="253" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:64" ht="18.75" customHeight="1">
       <c r="B253" t="s">
         <v>1139</v>
       </c>
@@ -53919,7 +53919,7 @@
         <v>[39.75305,-104.99995],</v>
       </c>
     </row>
-    <row r="254" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:64" ht="18.75" customHeight="1">
       <c r="B254" t="s">
         <v>217</v>
       </c>
@@ -54113,7 +54113,7 @@
       </c>
       <c r="BL254" s="7"/>
     </row>
-    <row r="255" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:64" ht="18.75" customHeight="1">
       <c r="B255" t="s">
         <v>218</v>
       </c>
@@ -54307,7 +54307,7 @@
       </c>
       <c r="BL255" s="7"/>
     </row>
-    <row r="256" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:64" ht="18.75" customHeight="1">
       <c r="B256" t="s">
         <v>1224</v>
       </c>
@@ -54509,7 +54509,7 @@
       </c>
       <c r="BL256" s="7"/>
     </row>
-    <row r="257" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:64" ht="18.75" customHeight="1">
       <c r="B257" t="s">
         <v>1222</v>
       </c>
@@ -54703,7 +54703,7 @@
       </c>
       <c r="BL257" s="7"/>
     </row>
-    <row r="258" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:64" ht="18.75" customHeight="1">
       <c r="B258" t="s">
         <v>145</v>
       </c>
@@ -54909,7 +54909,7 @@
       </c>
       <c r="BL258" s="7"/>
     </row>
-    <row r="259" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:64" ht="18.75" customHeight="1">
       <c r="B259" t="s">
         <v>146</v>
       </c>
@@ -55115,7 +55115,7 @@
       </c>
       <c r="BL259" s="7"/>
     </row>
-    <row r="260" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:64" ht="18.75" customHeight="1">
       <c r="B260" t="s">
         <v>219</v>
       </c>
@@ -55309,7 +55309,7 @@
       </c>
       <c r="BL260" s="7"/>
     </row>
-    <row r="261" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:64" ht="18.75" customHeight="1">
       <c r="B261" t="s">
         <v>147</v>
       </c>
@@ -55518,7 +55518,7 @@
       </c>
       <c r="BL261" s="7"/>
     </row>
-    <row r="262" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:64" ht="18.75" customHeight="1">
       <c r="B262" t="s">
         <v>881</v>
       </c>
@@ -55678,7 +55678,7 @@
         <v/>
       </c>
     </row>
-    <row r="263" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:64" ht="18.75" customHeight="1">
       <c r="B263" t="s">
         <v>148</v>
       </c>
@@ -55872,7 +55872,7 @@
       </c>
       <c r="BL263" s="7"/>
     </row>
-    <row r="264" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:64" ht="18.75" customHeight="1">
       <c r="B264" t="s">
         <v>149</v>
       </c>
@@ -56069,7 +56069,7 @@
       </c>
       <c r="BL264" s="7"/>
     </row>
-    <row r="265" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:64" ht="18.75" customHeight="1">
       <c r="B265" t="s">
         <v>150</v>
       </c>
@@ -56263,7 +56263,7 @@
       </c>
       <c r="BL265" s="7"/>
     </row>
-    <row r="266" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:64" ht="18.75" customHeight="1">
       <c r="B266" t="s">
         <v>1112</v>
       </c>
@@ -56419,7 +56419,7 @@
         <v>[39.77126,-105.044258],</v>
       </c>
     </row>
-    <row r="267" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:64" ht="18.75" customHeight="1">
       <c r="B267" t="s">
         <v>220</v>
       </c>
@@ -56613,7 +56613,7 @@
       </c>
       <c r="BL267" s="7"/>
     </row>
-    <row r="268" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:64" ht="18.75" customHeight="1">
       <c r="B268" t="s">
         <v>221</v>
       </c>
@@ -56807,7 +56807,7 @@
       </c>
       <c r="BL268" s="7"/>
     </row>
-    <row r="269" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:64" ht="18.75" customHeight="1">
       <c r="B269" t="s">
         <v>151</v>
       </c>
@@ -57001,7 +57001,7 @@
       </c>
       <c r="BL269" s="7"/>
     </row>
-    <row r="270" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:64" ht="18.75" customHeight="1">
       <c r="B270" t="s">
         <v>222</v>
       </c>
@@ -57195,7 +57195,7 @@
       </c>
       <c r="BL270" s="7"/>
     </row>
-    <row r="271" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:64" ht="18.75" customHeight="1">
       <c r="B271" t="s">
         <v>152</v>
       </c>
@@ -57401,7 +57401,7 @@
       </c>
       <c r="BL271" s="7"/>
     </row>
-    <row r="272" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:64" ht="18.75" customHeight="1">
       <c r="B272" t="s">
         <v>223</v>
       </c>
@@ -57565,7 +57565,7 @@
       </c>
       <c r="BL272" s="7"/>
     </row>
-    <row r="273" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:64" ht="18.75" customHeight="1">
       <c r="B273" t="s">
         <v>836</v>
       </c>
@@ -57770,7 +57770,7 @@
         <v/>
       </c>
     </row>
-    <row r="274" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:64" ht="18.75" customHeight="1">
       <c r="B274" t="s">
         <v>942</v>
       </c>
@@ -57975,7 +57975,7 @@
         <v/>
       </c>
     </row>
-    <row r="275" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:64" ht="18.75" customHeight="1">
       <c r="B275" t="s">
         <v>1256</v>
       </c>
@@ -58173,7 +58173,7 @@
         <v>[39.75305,-104.99995],</v>
       </c>
     </row>
-    <row r="276" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:64" ht="18.75" customHeight="1">
       <c r="B276" t="s">
         <v>235</v>
       </c>
@@ -58361,7 +58361,7 @@
       </c>
       <c r="BL276" s="7"/>
     </row>
-    <row r="277" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:64" ht="18.75" customHeight="1">
       <c r="B277" t="s">
         <v>902</v>
       </c>
@@ -58560,7 +58560,7 @@
         <v/>
       </c>
     </row>
-    <row r="278" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:64" ht="18.75" customHeight="1">
       <c r="B278" t="s">
         <v>910</v>
       </c>
@@ -58750,7 +58750,7 @@
         <v/>
       </c>
     </row>
-    <row r="279" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:64" ht="18.75" customHeight="1">
       <c r="B279" t="s">
         <v>830</v>
       </c>
@@ -58955,7 +58955,7 @@
         <v/>
       </c>
     </row>
-    <row r="280" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:64" ht="18.75" customHeight="1">
       <c r="B280" t="s">
         <v>244</v>
       </c>
@@ -59152,7 +59152,7 @@
       </c>
       <c r="BL280" s="7"/>
     </row>
-    <row r="281" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:64" ht="18.75" customHeight="1">
       <c r="B281" t="s">
         <v>865</v>
       </c>
@@ -59357,7 +59357,7 @@
         <v/>
       </c>
     </row>
-    <row r="282" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:64" ht="18.75" customHeight="1">
       <c r="B282" t="s">
         <v>918</v>
       </c>
@@ -59562,7 +59562,7 @@
         <v/>
       </c>
     </row>
-    <row r="283" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:64" ht="18.75" customHeight="1">
       <c r="B283" t="s">
         <v>153</v>
       </c>
@@ -59765,7 +59765,7 @@
       </c>
       <c r="BL283" s="7"/>
     </row>
-    <row r="284" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:64" ht="18.75" customHeight="1">
       <c r="B284" t="s">
         <v>944</v>
       </c>
@@ -59970,7 +59970,7 @@
         <v/>
       </c>
     </row>
-    <row r="285" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:64" ht="18.75" customHeight="1">
       <c r="B285" t="s">
         <v>879</v>
       </c>
@@ -60169,7 +60169,7 @@
         <v/>
       </c>
     </row>
-    <row r="286" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:64" ht="18.75" customHeight="1">
       <c r="B286" t="s">
         <v>154</v>
       </c>
@@ -60375,7 +60375,7 @@
       </c>
       <c r="BL286" s="7"/>
     </row>
-    <row r="287" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:64" ht="18.75" customHeight="1">
       <c r="B287" t="s">
         <v>238</v>
       </c>
@@ -60584,7 +60584,7 @@
       </c>
       <c r="BL287" s="7"/>
     </row>
-    <row r="288" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:64" ht="18.75" customHeight="1">
       <c r="B288" t="s">
         <v>155</v>
       </c>
@@ -60790,7 +60790,7 @@
       </c>
       <c r="BL288" s="7"/>
     </row>
-    <row r="289" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:64" ht="18.75" customHeight="1">
       <c r="B289" t="s">
         <v>156</v>
       </c>
@@ -60984,7 +60984,7 @@
       </c>
       <c r="BL289" s="7"/>
     </row>
-    <row r="290" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:64" ht="18.75" customHeight="1">
       <c r="B290" t="s">
         <v>224</v>
       </c>
@@ -61145,7 +61145,7 @@
       </c>
       <c r="BL290" s="7"/>
     </row>
-    <row r="291" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:64" ht="18.75" customHeight="1">
       <c r="B291" t="s">
         <v>225</v>
       </c>
@@ -61336,7 +61336,7 @@
       </c>
       <c r="BL291" s="7"/>
     </row>
-    <row r="292" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:64" ht="18.75" customHeight="1">
       <c r="B292" t="s">
         <v>928</v>
       </c>
@@ -61487,7 +61487,7 @@
         <v/>
       </c>
     </row>
-    <row r="293" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:64" ht="18.75" customHeight="1">
       <c r="B293" t="s">
         <v>157</v>
       </c>
@@ -61687,7 +61687,7 @@
       </c>
       <c r="BL293" s="7"/>
     </row>
-    <row r="294" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:64" ht="18.75" customHeight="1">
       <c r="B294" t="s">
         <v>924</v>
       </c>
@@ -61847,7 +61847,7 @@
         <v/>
       </c>
     </row>
-    <row r="295" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:64" ht="18.75" customHeight="1">
       <c r="B295" t="s">
         <v>226</v>
       </c>
@@ -62041,7 +62041,7 @@
       </c>
       <c r="BL295" s="7"/>
     </row>
-    <row r="296" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:64" ht="18.75" customHeight="1">
       <c r="B296" t="s">
         <v>1172</v>
       </c>
@@ -62242,7 +62242,7 @@
         <v>[39.72741,-104.98388],</v>
       </c>
     </row>
-    <row r="297" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:64" ht="18.75" customHeight="1">
       <c r="B297" t="s">
         <v>158</v>
       </c>
@@ -62436,7 +62436,7 @@
       </c>
       <c r="BL297" s="7"/>
     </row>
-    <row r="298" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:64" ht="18.75" customHeight="1">
       <c r="B298" t="s">
         <v>227</v>
       </c>
@@ -62633,7 +62633,7 @@
       </c>
       <c r="BL298" s="7"/>
     </row>
-    <row r="299" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:64" ht="18.75" customHeight="1">
       <c r="B299" t="s">
         <v>228</v>
       </c>
@@ -62827,7 +62827,7 @@
       </c>
       <c r="BL299" s="7"/>
     </row>
-    <row r="300" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:64" ht="18.75" customHeight="1">
       <c r="B300" t="s">
         <v>1257</v>
       </c>
@@ -63019,7 +63019,7 @@
         <v>[39.77142,-105.04415],</v>
       </c>
     </row>
-    <row r="301" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:64" ht="18.75" customHeight="1">
       <c r="B301" t="s">
         <v>229</v>
       </c>
@@ -63213,7 +63213,7 @@
       </c>
       <c r="BL301" s="7"/>
     </row>
-    <row r="302" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:64" ht="18.75" customHeight="1">
       <c r="B302" t="s">
         <v>159</v>
       </c>
@@ -63410,7 +63410,7 @@
       </c>
       <c r="BL302" s="7"/>
     </row>
-    <row r="303" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:64" ht="18.75" customHeight="1">
       <c r="B303" t="s">
         <v>160</v>
       </c>
@@ -63616,7 +63616,7 @@
       </c>
       <c r="BL303" s="7"/>
     </row>
-    <row r="304" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:64" ht="18.75" customHeight="1">
       <c r="B304" t="s">
         <v>885</v>
       </c>
@@ -63821,7 +63821,7 @@
         <v/>
       </c>
     </row>
-    <row r="305" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:64" ht="18.75" customHeight="1">
       <c r="B305" t="s">
         <v>254</v>
       </c>
@@ -63985,7 +63985,7 @@
       </c>
       <c r="BL305" s="7"/>
     </row>
-    <row r="306" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:64" ht="18.75" customHeight="1">
       <c r="B306" t="s">
         <v>932</v>
       </c>
@@ -64187,7 +64187,7 @@
         <v/>
       </c>
     </row>
-    <row r="307" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:64" ht="18.75" customHeight="1">
       <c r="B307" t="s">
         <v>161</v>
       </c>
@@ -64351,7 +64351,7 @@
       </c>
       <c r="BL307" s="7"/>
     </row>
-    <row r="308" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:64" ht="18.75" customHeight="1">
       <c r="B308" t="s">
         <v>1255</v>
       </c>
@@ -64531,7 +64531,7 @@
         <v>[39.74352,-104.96954],</v>
       </c>
     </row>
-    <row r="309" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:64" ht="18.75" customHeight="1">
       <c r="B309" t="s">
         <v>948</v>
       </c>
@@ -64730,7 +64730,7 @@
         <v/>
       </c>
     </row>
-    <row r="310" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:64" ht="18.75" customHeight="1">
       <c r="B310" t="s">
         <v>230</v>
       </c>
@@ -64924,7 +64924,7 @@
       </c>
       <c r="BL310" s="7"/>
     </row>
-    <row r="311" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:64" ht="18.75" customHeight="1">
       <c r="B311" t="s">
         <v>887</v>
       </c>
@@ -65129,7 +65129,7 @@
         <v/>
       </c>
     </row>
-    <row r="312" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:64" ht="18.75" customHeight="1">
       <c r="B312" t="s">
         <v>162</v>
       </c>
@@ -65323,7 +65323,7 @@
       </c>
       <c r="BL312" s="7"/>
     </row>
-    <row r="313" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:64" ht="18.75" customHeight="1">
       <c r="B313" t="s">
         <v>163</v>
       </c>
@@ -65529,7 +65529,7 @@
       </c>
       <c r="BL313" s="7"/>
     </row>
-    <row r="314" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:64" ht="18.75" customHeight="1">
       <c r="B314" t="s">
         <v>920</v>
       </c>
@@ -65734,7 +65734,7 @@
         <v/>
       </c>
     </row>
-    <row r="315" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:64" ht="18.75" customHeight="1">
       <c r="B315" t="s">
         <v>257</v>
       </c>
@@ -65898,7 +65898,7 @@
       </c>
       <c r="BL315" s="7"/>
     </row>
-    <row r="316" spans="2:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:64" ht="18.75" customHeight="1">
       <c r="B316" t="s">
         <v>164</v>
       </c>
@@ -66093,29 +66093,29 @@
       <c r="BL316" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C290"/>
-  <sortState ref="B2:BL315">
+  <autoFilter ref="C1:C290" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:BL315">
     <sortCondition ref="B2:B315"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="AR210" r:id="rId1"/>
-    <hyperlink ref="B24" r:id="rId2" display="https://www.yelp.com/biz/backstreet-tavern-and-grill-aurora?osq=Happy+Hour"/>
-    <hyperlink ref="B133" r:id="rId3" display="https://www.yelp.com/biz/improper-city-denver?osq=Happy+Hour"/>
-    <hyperlink ref="B182" r:id="rId4" display="https://www.yelp.com/biz/neighbors-denver?osq=Happy+Hour"/>
-    <hyperlink ref="AR279" r:id="rId5"/>
-    <hyperlink ref="AR78" r:id="rId6"/>
-    <hyperlink ref="AR311" r:id="rId7"/>
-    <hyperlink ref="AR277" r:id="rId8"/>
-    <hyperlink ref="AR187" r:id="rId9"/>
-    <hyperlink ref="AR284" r:id="rId10"/>
-    <hyperlink ref="G52" r:id="rId11" display="https://www.google.com/maps/place/Candlelight+Tavern/@39.709632,-104.9828235,17z/data=!4m5!3m4!1s0x876c7ee345a86e4d:0x6a6cf93c603a839b!8m2!3d39.709632!4d-104.9806348"/>
-    <hyperlink ref="AR199" r:id="rId12" tooltip="Osteria Marco" display="http://www.osteriamarco.com/"/>
-    <hyperlink ref="AR202" r:id="rId13" tooltip="Park Burger" display="http://parkburger.com/"/>
-    <hyperlink ref="AR9" r:id="rId14" tooltip="Acorn" display="http://www.denveracorn.com/"/>
-    <hyperlink ref="AR197" r:id="rId15"/>
-    <hyperlink ref="AR152" r:id="rId16"/>
-    <hyperlink ref="AR137" r:id="rId17"/>
-    <hyperlink ref="AR87" r:id="rId18"/>
+    <hyperlink ref="AR210" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B24" r:id="rId2" display="https://www.yelp.com/biz/backstreet-tavern-and-grill-aurora?osq=Happy+Hour" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B133" r:id="rId3" display="https://www.yelp.com/biz/improper-city-denver?osq=Happy+Hour" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B182" r:id="rId4" display="https://www.yelp.com/biz/neighbors-denver?osq=Happy+Hour" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="AR279" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="AR78" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="AR311" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="AR277" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="AR187" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="AR284" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G52" r:id="rId11" display="https://www.google.com/maps/place/Candlelight+Tavern/@39.709632,-104.9828235,17z/data=!4m5!3m4!1s0x876c7ee345a86e4d:0x6a6cf93c603a839b!8m2!3d39.709632!4d-104.9806348" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="AR199" r:id="rId12" tooltip="Osteria Marco" display="http://www.osteriamarco.com/" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="AR202" r:id="rId13" tooltip="Park Burger" display="http://parkburger.com/" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="AR9" r:id="rId14" tooltip="Acorn" display="http://www.denveracorn.com/" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="AR197" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="AR152" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="AR137" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="AR87" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -66123,16 +66123,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3:K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>1191</v>
       </c>
@@ -66155,7 +66155,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>39.755760000000002</v>
       </c>
@@ -66196,7 +66196,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>39.732250000000001</v>
       </c>
@@ -66234,7 +66234,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>39.754260000000002</v>
       </c>
@@ -66272,7 +66272,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>39.725490000000001</v>
       </c>
@@ -66310,7 +66310,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>39.753819999999997</v>
       </c>
@@ -66348,7 +66348,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>39.709600000000002</v>
       </c>
@@ -66386,7 +66386,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>39.76211</v>
       </c>
@@ -66424,7 +66424,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>39.748190000000001</v>
       </c>
@@ -66444,7 +66444,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>39.759590000000003</v>
       </c>
@@ -66464,7 +66464,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>39.727409999999999</v>
       </c>
@@ -66484,7 +66484,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>39.763539999999999</v>
       </c>
@@ -66504,7 +66504,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>39.768740000000001</v>
       </c>
@@ -66524,7 +66524,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>39.751339999999999</v>
       </c>
@@ -66544,7 +66544,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>39.717610000000001</v>
       </c>

</xml_diff>